<commit_message>
I found SQLite for Unity
is this our new save data system?
</commit_message>
<xml_diff>
--- a/Assets/Documents/Credit.xlsx
+++ b/Assets/Documents/Credit.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122D2C7E-B1F3-44A9-B8BD-CDCB9C32035E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715BB6BE-EEF4-47F9-8DAC-6511D841EE22}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Referensi" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Penulis</t>
   </si>
@@ -63,6 +63,18 @@
   </si>
   <si>
     <t>[100%]</t>
+  </si>
+  <si>
+    <t>Adorable73</t>
+  </si>
+  <si>
+    <t>https://answers.unity.com/questions/743400/database-sqlite-setup-for-unity.html</t>
+  </si>
+  <si>
+    <t>SQLite in Unity</t>
+  </si>
+  <si>
+    <t>Setup SQLite in Unity tutorial</t>
   </si>
 </sst>
 </file>
@@ -391,16 +403,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="3" width="58.44140625" customWidth="1"/>
+    <col min="2" max="2" width="75.77734375" customWidth="1"/>
+    <col min="3" max="3" width="58.44140625" customWidth="1"/>
     <col min="4" max="4" width="55" customWidth="1"/>
   </cols>
   <sheetData>
@@ -430,6 +443,20 @@
       </c>
       <c r="D2" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -444,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F5982EF-6D54-4DFF-84A0-34B808DCE994}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Tetrahedron and Non convex collider
blender tetrahedron is best. also never open excell file to Collab.

also script non convex collider is rough!

just convex mesh collider the tetrahedron and is enough just enough already!

do not open excell to Collab Unity! lockfile hinders other app to open the target excell xlsx
</commit_message>
<xml_diff>
--- a/Assets/Documents/Credit.xlsx
+++ b/Assets/Documents/Credit.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E8FDE9-B7DC-45A8-B08B-84138F088F53}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C690EB-7FA5-4D0E-B20C-AE6F395B87F7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Referensi" sheetId="1" r:id="rId1"/>
     <sheet name="Aset" sheetId="2" r:id="rId2"/>
+    <sheet name="Alat" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="61">
   <si>
     <t>Penulis</t>
   </si>
@@ -114,6 +115,96 @@
   </si>
   <si>
     <t>[&lt;100%]</t>
+  </si>
+  <si>
+    <t>https://gist.github.com/mynameisjacobj/8584bdc1e9e104b005044fdfda5fe9e5</t>
+  </si>
+  <si>
+    <t>mynamesisjacobj</t>
+  </si>
+  <si>
+    <t>Non Convex Mesh Collider</t>
+  </si>
+  <si>
+    <t>Unity tidak mendukun mesh collider non-cembung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unity Asset Collection </t>
+  </si>
+  <si>
+    <t>http://unityassetcollection.com/non-convex-mesh-collider-free-download/</t>
+  </si>
+  <si>
+    <t>[Bajakan] Non Convex Mesh Collider</t>
+  </si>
+  <si>
+    <t>[Tidak digunakan, larangan, dilarang bajakan] buat Mesh Collider cekung!</t>
+  </si>
+  <si>
+    <t>Productivity Boost</t>
+  </si>
+  <si>
+    <t>https://assetstore.unity.com/packages/tools/physics/non-convex-mesh-collider-84867</t>
+  </si>
+  <si>
+    <t>[ORI] Non Convex Mesh Collider</t>
+  </si>
+  <si>
+    <t>[Tidak digunakan, tidak gratis] buat Mesh Collider cekung!</t>
+  </si>
+  <si>
+    <t>[&gt;100%]</t>
+  </si>
+  <si>
+    <t>Free SFX</t>
+  </si>
+  <si>
+    <t>https://freesfx.co.uk/</t>
+  </si>
+  <si>
+    <t>Free SFX library</t>
+  </si>
+  <si>
+    <t>Pustaka efek suara gratis</t>
+  </si>
+  <si>
+    <t>Blender Foundation</t>
+  </si>
+  <si>
+    <t>https://www.blender.org</t>
+  </si>
+  <si>
+    <t>Blender 3D</t>
+  </si>
+  <si>
+    <t>Buat apapun 3D</t>
+  </si>
+  <si>
+    <t>https://www.unity3d.com</t>
+  </si>
+  <si>
+    <t>Unity Engine</t>
+  </si>
+  <si>
+    <t>buat game 2D atau 3D</t>
+  </si>
+  <si>
+    <t>cegaton</t>
+  </si>
+  <si>
+    <t>https://blender.stackexchange.com/questions/10725/how-do-i-create-an-equilateral-tetrahedron</t>
+  </si>
+  <si>
+    <t>Robin bets</t>
+  </si>
+  <si>
+    <t>Tetrahedron Blender</t>
+  </si>
+  <si>
+    <t>Buat dengan fungsi matematika</t>
+  </si>
+  <si>
+    <t>buat dengan sudut berlawanan</t>
   </si>
 </sst>
 </file>
@@ -442,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,6 +603,48 @@
         <v>25</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{8341CB2B-2293-45F0-88B5-43136C56BE15}"/>
@@ -522,17 +655,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F5982EF-6D54-4DFF-84A0-34B808DCE994}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="3" width="58.44140625" customWidth="1"/>
-    <col min="4" max="4" width="55" customWidth="1"/>
+    <col min="1" max="1" width="29.88671875" customWidth="1"/>
+    <col min="2" max="2" width="73.21875" customWidth="1"/>
+    <col min="3" max="3" width="58.44140625" customWidth="1"/>
+    <col min="4" max="4" width="62.33203125" customWidth="1"/>
     <col min="5" max="5" width="20.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -604,7 +738,135 @@
         <v>30</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{927B1521-9E15-4B36-BF38-84E29CC4BA22}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.88671875" customWidth="1"/>
+    <col min="2" max="2" width="73.21875" customWidth="1"/>
+    <col min="3" max="3" width="58.44140625" customWidth="1"/>
+    <col min="4" max="4" width="62.33203125" customWidth="1"/>
+    <col min="5" max="5" width="20.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{2B93406E-B914-4F7E-9D04-85AA8F1EDAE1}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{B4A70F25-0E74-4F6A-8780-C5CEFFE6BD3E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
blender tutorial & SHanpe moving
We learnt blender again and it is so many. just learn what we need instead.

also 3D version of Move character is way more different. we are learning milestone!
we need to know how to roll based on what camera sees ahead and slide based on what camera sees.
we need contraining deadzone. from the off the deadzone, it must be zero. We thought constraint. So benefiting many controller to add more velocity likely be removed here. deadzone is min and 1 is max I think. ahh.
</commit_message>
<xml_diff>
--- a/Assets/Documents/Credit.xlsx
+++ b/Assets/Documents/Credit.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C690EB-7FA5-4D0E-B20C-AE6F395B87F7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C936B6-7461-4E6B-AFB2-10171F4B8434}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="68">
   <si>
     <t>Penulis</t>
   </si>
@@ -205,6 +205,27 @@
   </si>
   <si>
     <t>buat dengan sudut berlawanan</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=PUSOg5YEflM</t>
+  </si>
+  <si>
+    <t>Pro Builder</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Pro Builder Perkenalan tutorial</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PLa1F2ddGya_8V90Kd5eC5PeBjySbXWGK1</t>
+  </si>
+  <si>
+    <t>Blender Fundamentals</t>
+  </si>
+  <si>
+    <t>Blender tutorial beginner lengkap</t>
   </si>
 </sst>
 </file>
@@ -533,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -547,7 +568,7 @@
     <col min="4" max="4" width="55" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -561,79 +582,82 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>24</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>44</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>45</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>46</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>55</v>
-      </c>
-      <c r="B6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>57</v>
       </c>
       <c r="B7" t="s">
         <v>56</v>
@@ -642,14 +666,44 @@
         <v>58</v>
       </c>
       <c r="D7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{8341CB2B-2293-45F0-88B5-43136C56BE15}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{8341CB2B-2293-45F0-88B5-43136C56BE15}"/>
+    <hyperlink ref="B2" r:id="rId2" display="https://www.bing.com/search?q=unity+probuilder&amp;form=EDGTCT&amp;qs=AS&amp;cvid=21509d34d4484303becc906eef91a8fb&amp;refig=a8e419fc3ce1430fe0c1388e8b2d3902&amp;cc=ID&amp;setlang=id-ID&amp;plvar=0&amp;PC=ASTS" xr:uid="{8888DA5E-20EE-497B-9CE3-679392D2E28C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
3rd person camera & Relative to cam movement
it works all!

we have frankensteined things up to these movements!!!

now move relative to camera direction!!!!

Praise the Lord, it works!!!
</commit_message>
<xml_diff>
--- a/Assets/Documents/Credit.xlsx
+++ b/Assets/Documents/Credit.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283F232F-FD5F-456C-84D0-DF5B5B27E135}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBA4AAA-AE83-47FD-9171-7C09972620BC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Referensi" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="131">
   <si>
     <t>Penulis</t>
   </si>
@@ -397,6 +397,30 @@
   </si>
   <si>
     <t>Interface Github gampang</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=xcn7hz7J7sI</t>
+  </si>
+  <si>
+    <t>Jayanam</t>
+  </si>
+  <si>
+    <t>Camera 3rd person mouse aim</t>
+  </si>
+  <si>
+    <t>kamera arah tetikus</t>
+  </si>
+  <si>
+    <t>Andrey Kubyshkin</t>
+  </si>
+  <si>
+    <t>https://forum.unity.com/threads/moving-character-relative-to-camera.383086/</t>
+  </si>
+  <si>
+    <t>Move character relative to camera</t>
+  </si>
+  <si>
+    <t>Gerakan karakter relative dengan arah hadapan kamera</t>
   </si>
 </sst>
 </file>
@@ -737,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -934,6 +958,34 @@
       </c>
       <c r="D13" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" t="s">
+        <v>125</v>
+      </c>
+      <c r="D14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D15" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1176,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{927B1521-9E15-4B36-BF38-84E29CC4BA22}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Hexagoned and Blender rant
Hexagon Engine progressed again

also rant to Blender Foundation for the Cloud is Blender's version of Patreon, locked up subscription
</commit_message>
<xml_diff>
--- a/Assets/Documents/Credit.xlsx
+++ b/Assets/Documents/Credit.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE444595-486D-49E5-B55C-782E1E0D74DF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D506834-9CA8-44EA-9E02-566192024E8D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,6 +12,11 @@
     <sheet name="Aset" sheetId="2" r:id="rId2"/>
     <sheet name="Alat" sheetId="4" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Alat!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Aset!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Referensi!$A$1:$D$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="168">
   <si>
     <t>Penulis</t>
   </si>
@@ -469,6 +474,69 @@
   </si>
   <si>
     <t>Buat GameObject tidak hancur saat loading</t>
+  </si>
+  <si>
+    <t>tutor4u</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=rZC8i7nq32k&amp;t=45s</t>
+  </si>
+  <si>
+    <t>Animating in Blender, Beginner</t>
+  </si>
+  <si>
+    <t>Dasar-dasar animasi di Blender</t>
+  </si>
+  <si>
+    <t>https://cloud.blender.org</t>
+  </si>
+  <si>
+    <t>Situs kumpulan proyek Blender (Free Trial termasuk)</t>
+  </si>
+  <si>
+    <t>per (default: Unit)</t>
+  </si>
+  <si>
+    <t>bulan</t>
+  </si>
+  <si>
+    <t>LaunchExcel</t>
+  </si>
+  <si>
+    <t>https://www.launchexcel.com/autofilter-keyboard-shortcut-video/</t>
+  </si>
+  <si>
+    <t>Autofilter excel</t>
+  </si>
+  <si>
+    <t>Filter otomatis Excel</t>
+  </si>
+  <si>
+    <t>[Ironis-Miris] Blender Cloud</t>
+  </si>
+  <si>
+    <t>gandalf3</t>
+  </si>
+  <si>
+    <t>https://blender.stackexchange.com/questions/15687/making-holes-in-a-mesh</t>
+  </si>
+  <si>
+    <t>Hole in Mesh</t>
+  </si>
+  <si>
+    <t>Buat lubang dalam Mesh</t>
+  </si>
+  <si>
+    <t>Chipper Videos</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=7UzABVPVXtM</t>
+  </si>
+  <si>
+    <t>Stretch video Kdenlive</t>
+  </si>
+  <si>
+    <t>Cara strectch video di Kdenlive</t>
   </si>
 </sst>
 </file>
@@ -478,7 +546,7 @@
   <numFmts count="1">
     <numFmt numFmtId="42" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -494,8 +562,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -505,6 +588,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -522,12 +611,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="42" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="42" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipertaut" xfId="1" builtinId="8"/>
@@ -809,16 +902,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="75.77734375" customWidth="1"/>
+    <col min="2" max="2" width="88.33203125" customWidth="1"/>
     <col min="3" max="3" width="58.44140625" customWidth="1"/>
     <col min="4" max="4" width="55" customWidth="1"/>
   </cols>
@@ -872,7 +965,7 @@
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C4" t="s">
@@ -886,7 +979,7 @@
       <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C5" t="s">
@@ -900,7 +993,7 @@
       <c r="A6" t="s">
         <v>43</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C6" t="s">
@@ -914,7 +1007,7 @@
       <c r="A7" t="s">
         <v>54</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C7" t="s">
@@ -928,7 +1021,7 @@
       <c r="A8" t="s">
         <v>56</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C8" t="s">
@@ -942,7 +1035,7 @@
       <c r="A9" t="s">
         <v>47</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C9" t="s">
@@ -970,7 +1063,7 @@
       <c r="A11" t="s">
         <v>71</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C11" t="s">
@@ -984,7 +1077,7 @@
       <c r="A12" t="s">
         <v>71</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C12" t="s">
@@ -998,7 +1091,7 @@
       <c r="A13" t="s">
         <v>87</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C13" t="s">
@@ -1012,7 +1105,7 @@
       <c r="A14" t="s">
         <v>124</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>123</v>
       </c>
       <c r="C14" t="s">
@@ -1026,7 +1119,7 @@
       <c r="A15" t="s">
         <v>127</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>128</v>
       </c>
       <c r="C15" t="s">
@@ -1040,7 +1133,7 @@
       <c r="A16" t="s">
         <v>131</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>132</v>
       </c>
       <c r="C16" t="s">
@@ -1054,7 +1147,7 @@
       <c r="A17" t="s">
         <v>135</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>136</v>
       </c>
       <c r="C17" t="s">
@@ -1068,7 +1161,7 @@
       <c r="A18" t="s">
         <v>138</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>139</v>
       </c>
       <c r="C18" t="s">
@@ -1082,7 +1175,7 @@
       <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>144</v>
       </c>
       <c r="C19" t="s">
@@ -1092,23 +1185,99 @@
         <v>146</v>
       </c>
     </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C20" t="s">
+        <v>149</v>
+      </c>
+      <c r="D20" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>155</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C21" t="s">
+        <v>157</v>
+      </c>
+      <c r="D21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>160</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C22" t="s">
+        <v>162</v>
+      </c>
+      <c r="D22" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>164</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C23" t="s">
+        <v>166</v>
+      </c>
+      <c r="D23" t="s">
+        <v>167</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:D1" xr:uid="{518CE555-9118-4462-942C-FA7E956AA36C}"/>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{8341CB2B-2293-45F0-88B5-43136C56BE15}"/>
     <hyperlink ref="B2" r:id="rId2" display="https://www.bing.com/search?q=unity+probuilder&amp;form=EDGTCT&amp;qs=AS&amp;cvid=21509d34d4484303becc906eef91a8fb&amp;refig=a8e419fc3ce1430fe0c1388e8b2d3902&amp;cc=ID&amp;setlang=id-ID&amp;plvar=0&amp;PC=ASTS" xr:uid="{8888DA5E-20EE-497B-9CE3-679392D2E28C}"/>
     <hyperlink ref="B10" r:id="rId3" display="https://www.bing.com/search?q=unity+arduino&amp;form=EDGTCT&amp;qs=AS&amp;cvid=994252eb30c24d75a8f449fe2da9e57b&amp;refig=b7058406c71b4c25b4d274b40bc530dc&amp;cc=ID&amp;setlang=id-ID&amp;plvar=0&amp;PC=ASTS" xr:uid="{9DB667AB-3576-4228-99AD-61E427039138}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{C3C3B09C-5DEB-4B8E-841C-70E0BB31853C}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{6988B4E2-DE3C-457D-B3F7-849EE0F3A545}"/>
+    <hyperlink ref="B6" r:id="rId6" xr:uid="{179C3F0F-11D5-4532-ACC3-64B06557D3E6}"/>
+    <hyperlink ref="B7" r:id="rId7" xr:uid="{E2754732-5A21-49BB-ADE4-C591E312644F}"/>
+    <hyperlink ref="B8" r:id="rId8" xr:uid="{7BBDF7E8-9AAD-4424-9471-29ACF701D104}"/>
+    <hyperlink ref="B9" r:id="rId9" xr:uid="{5B0145D8-357F-48D3-B248-62250CD2431B}"/>
+    <hyperlink ref="B11" r:id="rId10" location="54679189" xr:uid="{172E0F0D-F5C6-4BAB-9D86-8447F7C097A9}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{DBDDD647-1B6A-4151-AFF9-4D566AB66D66}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{BB7F0E62-F3DC-4412-9F52-B5C39B254A0C}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{B101E529-B316-4D74-8211-4BBF88BF731D}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{9B87494D-D37E-433C-8510-4481B52753E3}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{EDC5A6B3-DA4A-4662-A68B-E96386544B7D}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{F3DB1784-5D7E-47BA-8E83-2AFBFABEA496}"/>
+    <hyperlink ref="B18" r:id="rId17" xr:uid="{237CB907-76FD-4788-880B-AE9C0A3BAFB9}"/>
+    <hyperlink ref="B19" r:id="rId18" xr:uid="{360329DC-E504-436D-83F7-72BE2873ED28}"/>
+    <hyperlink ref="B20" r:id="rId19" xr:uid="{1549C7E2-EB18-4131-A032-4E94527D9883}"/>
+    <hyperlink ref="B21" r:id="rId20" xr:uid="{29097DAE-2D9C-4C70-A00A-9FB81094F203}"/>
+    <hyperlink ref="B22" r:id="rId21" xr:uid="{5C53E1C2-DBEB-4402-815D-39B0D71313E5}"/>
+    <hyperlink ref="B23" r:id="rId22" xr:uid="{E89A8F8F-5808-437A-8965-D98629B8DBC2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId23"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F5982EF-6D54-4DFF-84A0-34B808DCE994}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1119,9 +1288,10 @@
     <col min="4" max="4" width="62.33203125" customWidth="1"/>
     <col min="5" max="5" width="20.21875" customWidth="1"/>
     <col min="6" max="6" width="35.21875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1140,12 +1310,15 @@
       <c r="F1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C2" t="s">
@@ -1161,11 +1334,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C3" t="s">
@@ -1181,11 +1354,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C4" t="s">
@@ -1201,11 +1374,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C5" t="s">
@@ -1221,11 +1394,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -1242,11 +1415,11 @@
         <v>135000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1262,11 +1435,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>78</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>79</v>
       </c>
       <c r="C8" t="s">
@@ -1282,11 +1455,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>83</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>84</v>
       </c>
       <c r="C9" t="s">
@@ -1302,11 +1475,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>91</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C10" t="s">
@@ -1322,7 +1495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>103</v>
       </c>
@@ -1339,9 +1512,45 @@
         <v>0</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="8">
+        <v>160000</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:G1" xr:uid="{D4998491-F79F-4E20-AD30-35C229566CF5}"/>
+  <hyperlinks>
+    <hyperlink ref="B12" r:id="rId1" xr:uid="{90C255A6-433B-429B-AC09-4DA27AB53DC1}"/>
+    <hyperlink ref="B10" r:id="rId2" xr:uid="{E2682584-8BD1-452F-B20F-EA337EB8024A}"/>
+    <hyperlink ref="B9" r:id="rId3" xr:uid="{651C413D-37CD-4D11-96C8-3122ABE6AB22}"/>
+    <hyperlink ref="B8" r:id="rId4" xr:uid="{C4B7F807-26A1-4EE7-95B9-AF99406C2693}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{8865E3C4-F424-4A69-8749-47AF6F585A15}"/>
+    <hyperlink ref="B6" r:id="rId6" xr:uid="{7E8E5508-B77A-4112-A609-D4AB06DD23B4}"/>
+    <hyperlink ref="B5" r:id="rId7" xr:uid="{2A7B9AB8-B79F-41BA-944D-C033FD089E23}"/>
+    <hyperlink ref="B4" r:id="rId8" xr:uid="{BF25938B-055B-4C4B-8487-B6409C4DE457}"/>
+    <hyperlink ref="B3" r:id="rId9" xr:uid="{E1149810-C758-477C-9942-C4C33EB25921}"/>
+    <hyperlink ref="B2" r:id="rId10" xr:uid="{2464CB29-9F91-477E-8B13-01380045A292}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId11"/>
 </worksheet>
 </file>
 
@@ -1350,7 +1559,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1536,7 +1745,7 @@
       <c r="A11" t="s">
         <v>117</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>118</v>
       </c>
       <c r="C11" t="s">
@@ -1550,6 +1759,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E1" xr:uid="{906CCFA5-9A55-4898-8A4F-4996F8FCEFB4}"/>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{2B93406E-B914-4F7E-9D04-85AA8F1EDAE1}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{B4A70F25-0E74-4F6A-8780-C5CEFFE6BD3E}"/>
@@ -1559,6 +1769,7 @@
     <hyperlink ref="B7" r:id="rId6" xr:uid="{627A03C1-9C03-451E-A9C9-2F5FC22C9ED5}"/>
     <hyperlink ref="B8" r:id="rId7" xr:uid="{AF2171C5-9574-4AE4-871D-FA7A1EE1300E}"/>
     <hyperlink ref="B10" r:id="rId8" xr:uid="{E4A3B2C0-E265-41AA-85FB-647FA8D349F3}"/>
+    <hyperlink ref="B11" r:id="rId9" xr:uid="{76DF93BD-999D-4F5D-9CBB-7BEE07701AD8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Wiw me made film
Blender Cloud. what an irony
</commit_message>
<xml_diff>
--- a/Assets/Documents/Credit.xlsx
+++ b/Assets/Documents/Credit.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D506834-9CA8-44EA-9E02-566192024E8D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4C8C9F-6923-4E19-A16E-CFC0DC93C70C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="176">
   <si>
     <t>Penulis</t>
   </si>
@@ -537,6 +537,30 @@
   </si>
   <si>
     <t>Cara strectch video di Kdenlive</t>
+  </si>
+  <si>
+    <t>derHugo</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/55752495/unity-2019-1-0f2-blender-could-not-convert-the-blend-file-to-fbx-file</t>
+  </si>
+  <si>
+    <t>Unity 2019 import blender into FBX bug workaround</t>
+  </si>
+  <si>
+    <t>Unity 2019 terdapat masalah dengan impor Blender sebelum versi 2.8</t>
+  </si>
+  <si>
+    <t>Manash Kumar Mandal</t>
+  </si>
+  <si>
+    <t>https://blog.manash.me/serial-communication-with-an-arduino-using-c-on-windows-d08710186498</t>
+  </si>
+  <si>
+    <t>Arduino Serial communication C++</t>
+  </si>
+  <si>
+    <t>Komunikasi arduino menggunakan C++ melalui serial, buat Godot C++</t>
   </si>
 </sst>
 </file>
@@ -902,18 +926,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" customWidth="1"/>
     <col min="2" max="2" width="88.33203125" customWidth="1"/>
     <col min="3" max="3" width="58.44140625" customWidth="1"/>
-    <col min="4" max="4" width="55" customWidth="1"/>
+    <col min="4" max="4" width="59.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1239,6 +1263,34 @@
       </c>
       <c r="D23" t="s">
         <v>167</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>168</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C24" t="s">
+        <v>170</v>
+      </c>
+      <c r="D24" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>172</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C25" t="s">
+        <v>174</v>
+      </c>
+      <c r="D25" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -1266,9 +1318,11 @@
     <hyperlink ref="B21" r:id="rId20" xr:uid="{29097DAE-2D9C-4C70-A00A-9FB81094F203}"/>
     <hyperlink ref="B22" r:id="rId21" xr:uid="{5C53E1C2-DBEB-4402-815D-39B0D71313E5}"/>
     <hyperlink ref="B23" r:id="rId22" xr:uid="{E89A8F8F-5808-437A-8965-D98629B8DBC2}"/>
+    <hyperlink ref="B24" r:id="rId23" xr:uid="{53E47B73-95BD-4621-AFA8-AB441A3721F0}"/>
+    <hyperlink ref="B25" r:id="rId24" xr:uid="{C1F73AF8-7AD1-45AE-9C38-E427FA6FE6BB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId23"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId25"/>
 </worksheet>
 </file>
 

</xml_diff>